<commit_message>
Updated my (Alex) estimated completion dates
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
   <si>
     <t>Item</t>
   </si>
@@ -113,9 +113,6 @@
     <t>OData Core – Appendix – XSD for CSDL</t>
   </si>
   <si>
-    <t>URI - XXX</t>
-  </si>
-  <si>
     <t>Atom - XXX</t>
   </si>
   <si>
@@ -141,6 +138,18 @@
   </si>
   <si>
     <t>JSON (with metadata) - XXX</t>
+  </si>
+  <si>
+    <t>URI - Components / Service Root</t>
+  </si>
+  <si>
+    <t>URI - Addressing - Entities/ Properties / Values / Links</t>
+  </si>
+  <si>
+    <t>URI - Query Options</t>
+  </si>
+  <si>
+    <t>URI - Addressing - SOPS, Actions, Functions</t>
   </si>
 </sst>
 </file>
@@ -148,9 +157,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="m/d;@"/>
+    <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +171,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -190,22 +215,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -214,8 +241,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -515,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +603,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -578,7 +617,7 @@
         <v>11</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -592,7 +631,7 @@
         <v>40921</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -603,7 +642,7 @@
         <v>15</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -614,7 +653,7 @@
         <v>10</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -625,7 +664,7 @@
         <v>18</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -636,7 +675,7 @@
         <v>18</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -647,7 +686,7 @@
         <v>18</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -657,8 +696,11 @@
       <c r="B10" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="C10" s="5">
+        <v>40975</v>
+      </c>
       <c r="G10" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -669,7 +711,7 @@
         <v>24</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -677,7 +719,7 @@
         <v>25</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -687,8 +729,11 @@
       <c r="B13" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="C13" s="5">
+        <v>40949</v>
+      </c>
       <c r="G13" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -698,16 +743,25 @@
       <c r="B14" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="C14" s="5">
+        <v>40954</v>
+      </c>
       <c r="G14" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
+      <c r="B15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="5">
+        <v>40956</v>
+      </c>
       <c r="G15" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -715,7 +769,7 @@
         <v>29</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -723,7 +777,7 @@
         <v>30</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -731,62 +785,119 @@
         <v>31</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="7" t="s">
+      <c r="A19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>36</v>
+      <c r="C19" s="10">
+        <v>40959</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>36</v>
+      <c r="A20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="10">
+        <v>40963</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>36</v>
+      <c r="A21" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="10">
+        <v>40968</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>36</v>
+      <c r="A22" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="10">
+        <v>40970</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>36</v>
+      <c r="G26" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -815,27 +926,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
results of sync meeting
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="61">
   <si>
     <t>Item</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>OData Core</t>
-  </si>
-  <si>
     <t>OData Core - Overview</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>MikeF</t>
   </si>
   <si>
-    <t>OData Core - Terminology</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
@@ -95,33 +89,18 @@
     <t>OData Core – Interaction Semantics – Data  Modification</t>
   </si>
   <si>
-    <t>OData Core – Interaction Semantics – Actions</t>
-  </si>
-  <si>
     <t>OData Core – Interaction Semantics – Functions</t>
   </si>
   <si>
     <t>OData Core – Interaction Semantics – Service Ops</t>
   </si>
   <si>
-    <t>OData Core – Interaction Semantics – Batch Costs</t>
-  </si>
-  <si>
     <t>OData Core – Appendix  – Formal CSDL description</t>
   </si>
   <si>
     <t>OData Core – Appendix – XSD for CSDL</t>
   </si>
   <si>
-    <t>Atom - XXX</t>
-  </si>
-  <si>
-    <t>JSON - XXX</t>
-  </si>
-  <si>
-    <t>Batch - XXX</t>
-  </si>
-  <si>
     <t>Not Started</t>
   </si>
   <si>
@@ -137,19 +116,88 @@
     <t>Complete</t>
   </si>
   <si>
-    <t>JSON (with metadata) - XXX</t>
-  </si>
-  <si>
-    <t>URI - Components / Service Root</t>
-  </si>
-  <si>
-    <t>URI - Addressing - Entities/ Properties / Values / Links</t>
-  </si>
-  <si>
-    <t>URI - Query Options</t>
-  </si>
-  <si>
     <t>URI - Addressing - SOPS, Actions, Functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batch </t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>alexj</t>
+  </si>
+  <si>
+    <t>mflasko</t>
+  </si>
+  <si>
+    <t>Alex/MikeF</t>
+  </si>
+  <si>
+    <t>OData Core – Interaction Semantics – Actions no examples</t>
+  </si>
+  <si>
+    <t>OData Core – Interaction Semantics – Actions examples</t>
+  </si>
+  <si>
+    <t>Atom Format</t>
+  </si>
+  <si>
+    <t>JSON (classic version)</t>
+  </si>
+  <si>
+    <t>Pablo</t>
+  </si>
+  <si>
+    <t>MarkS</t>
+  </si>
+  <si>
+    <t>MarkS (MikeP/F backups)</t>
+  </si>
+  <si>
+    <t>MFlasko</t>
+  </si>
+  <si>
+    <t>JSON Format (efficient format) + its vocab</t>
+  </si>
+  <si>
+    <t>OData Core - Glossary</t>
+  </si>
+  <si>
+    <t>URI glossary terms (service root, etc)</t>
+  </si>
+  <si>
+    <t>AlexJ</t>
+  </si>
+  <si>
+    <t>URI - Addressing conventions (consider using odata.org as base)</t>
+  </si>
+  <si>
+    <t>Mflasko, Arlo</t>
+  </si>
+  <si>
+    <t>Pablo, MikeP</t>
+  </si>
+  <si>
+    <t>Andy</t>
+  </si>
+  <si>
+    <t>Mflasko</t>
+  </si>
+  <si>
+    <t>Work Items</t>
+  </si>
+  <si>
+    <t>Create table of doc names and short ref tags</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>mflasko / pablo</t>
+  </si>
+  <si>
+    <t>pablo</t>
   </si>
 </sst>
 </file>
@@ -220,7 +268,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -251,13 +299,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -554,18 +653,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="12" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="4" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="5" customWidth="1"/>
     <col min="6" max="6" width="20" style="5" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" style="4" customWidth="1"/>
@@ -602,36 +701,60 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
+      <c r="B2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="G2" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C3" s="5">
+        <v>40952</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5">
-        <v>40921</v>
+      <c r="C4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -639,21 +762,39 @@
         <v>14</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>10</v>
+      <c r="C6" s="5">
+        <v>40956</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="5">
+        <v>40959</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -661,32 +802,59 @@
         <v>17</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="C7" s="5">
+        <v>40956</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="5">
+        <v>40959</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="C8" s="5">
+        <v>40954</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="5">
+        <v>40959</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>18</v>
+        <v>38</v>
+      </c>
+      <c r="C9" s="5">
+        <v>40946</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="5">
+        <v>40952</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -696,11 +864,17 @@
       <c r="B10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="5">
-        <v>40975</v>
+      <c r="C10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -708,199 +882,313 @@
         <v>23</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>24</v>
+        <v>9</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>39</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="5">
+        <v>40959</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="5">
-        <v>40949</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>35</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="10">
+        <v>40954</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="10">
+        <v>40959</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="9" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14" s="5">
         <v>40954</v>
       </c>
+      <c r="D14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="5">
+        <v>40964</v>
+      </c>
       <c r="G14" s="4" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="5">
         <v>40956</v>
       </c>
+      <c r="D15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="10">
+        <v>40964</v>
+      </c>
       <c r="G15" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="5">
+        <v>40968</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="5">
+        <v>40971</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="10">
+        <v>40968</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>35</v>
+      <c r="A18" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="10">
+        <v>40959</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="10">
+        <v>40962</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C19" s="10">
-        <v>40959</v>
-      </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+        <v>40963</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="10">
+        <v>40962</v>
+      </c>
       <c r="F19" s="8"/>
       <c r="G19" s="9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C20" s="10">
-        <v>40963</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+        <v>40968</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="F20" s="8"/>
       <c r="G20" s="9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="10">
-        <v>40968</v>
-      </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="9" t="s">
-        <v>35</v>
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="5">
+        <v>40963</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="5">
+        <v>40966</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="10">
-        <v>40970</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="9" t="s">
-        <v>35</v>
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="C24" s="5">
+        <v>40954</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>35</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="5">
+        <v>40953</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Not Started"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -926,27 +1214,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated status of versioning and extensibility.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="61">
   <si>
     <t>Item</t>
   </si>
@@ -306,21 +306,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -331,21 +317,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -656,7 +628,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,8 +756,8 @@
       <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="5">
-        <v>40956</v>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>37</v>
@@ -804,8 +776,8 @@
       <c r="B7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="5">
-        <v>40956</v>
+      <c r="C7" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>36</v>
@@ -1179,13 +1151,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
batch updates and feedback from doc sync meeting.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -4,18 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20160" windowHeight="8100" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
     <sheet name="status" sheetId="2" r:id="rId2"/>
+    <sheet name="Document Names &amp; Abbreviations" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">schedule!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="79">
   <si>
     <t>Item</t>
   </si>
@@ -143,18 +147,12 @@
     <t>Atom Format</t>
   </si>
   <si>
-    <t>JSON (classic version)</t>
-  </si>
-  <si>
     <t>Pablo</t>
   </si>
   <si>
     <t>MarkS</t>
   </si>
   <si>
-    <t>MarkS (MikeP/F backups)</t>
-  </si>
-  <si>
     <t>MFlasko</t>
   </si>
   <si>
@@ -198,6 +196,66 @@
   </si>
   <si>
     <t>pablo</t>
+  </si>
+  <si>
+    <t>MarkS (MikeP - 2 initial sections)</t>
+  </si>
+  <si>
+    <t>JSON (verbose version)</t>
+  </si>
+  <si>
+    <t>Document Names</t>
+  </si>
+  <si>
+    <t>Abbreviations</t>
+  </si>
+  <si>
+    <t>Open Data Protocol</t>
+  </si>
+  <si>
+    <t>[OData:Core]</t>
+  </si>
+  <si>
+    <t>OData: AtomPub Format</t>
+  </si>
+  <si>
+    <t>[OData:AtomPub]</t>
+  </si>
+  <si>
+    <t>OData: JSON Verbose Format</t>
+  </si>
+  <si>
+    <t>OData: JSON</t>
+  </si>
+  <si>
+    <t>[OData:JSON]</t>
+  </si>
+  <si>
+    <t>[OData:JSONVerbose]</t>
+  </si>
+  <si>
+    <t>[OData:Batch]</t>
+  </si>
+  <si>
+    <t>OData: Batch Processing</t>
+  </si>
+  <si>
+    <t>Relative URLs to the Docs</t>
+  </si>
+  <si>
+    <t>&lt;some base&gt;/atom</t>
+  </si>
+  <si>
+    <t>&lt;some base&gt;/jsonverbose</t>
+  </si>
+  <si>
+    <t>&lt;some base&gt;/json</t>
+  </si>
+  <si>
+    <t>&lt;some base&gt;/batch</t>
+  </si>
+  <si>
+    <t>&lt;some base&gt;/odata</t>
   </si>
 </sst>
 </file>
@@ -306,21 +364,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -331,21 +375,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -655,14 +685,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="5" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" style="4" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="5" customWidth="1"/>
@@ -708,7 +738,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>35</v>
@@ -725,21 +755,21 @@
         <v>12</v>
       </c>
       <c r="C3" s="5">
-        <v>40952</v>
+        <v>40956</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>35</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>13</v>
@@ -765,16 +795,16 @@
         <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E5" s="5">
+        <v>40956</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -794,7 +824,7 @@
         <v>40959</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -814,7 +844,7 @@
         <v>40959</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -825,7 +855,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="5">
-        <v>40954</v>
+        <v>40955</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>16</v>
@@ -854,7 +884,7 @@
         <v>40952</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -868,7 +898,7 @@
         <v>35</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>35</v>
@@ -884,17 +914,17 @@
       <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>35</v>
+      <c r="C11" s="5">
+        <v>40970</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>35</v>
+        <v>44</v>
+      </c>
+      <c r="E11" s="5">
+        <v>40976</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -914,7 +944,7 @@
         <v>40959</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -925,7 +955,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="10">
-        <v>40954</v>
+        <v>40956</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>16</v>
@@ -935,7 +965,7 @@
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -946,7 +976,7 @@
         <v>20</v>
       </c>
       <c r="C14" s="5">
-        <v>40954</v>
+        <v>40956</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>16</v>
@@ -955,7 +985,7 @@
         <v>40964</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -983,7 +1013,7 @@
         <v>26</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C16" s="5">
         <v>40968</v>
@@ -1003,7 +1033,7 @@
         <v>27</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="10">
         <v>40968</v>
@@ -1020,16 +1050,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" s="10">
         <v>40959</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E18" s="10">
         <v>40962</v>
@@ -1041,16 +1071,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C19" s="10">
         <v>40963</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E19" s="10">
         <v>40962</v>
@@ -1065,7 +1095,7 @@
         <v>33</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C20" s="10">
         <v>40968</v>
@@ -1092,18 +1122,18 @@
         <v>40963</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E21" s="5">
         <v>40966</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>9</v>
@@ -1112,7 +1142,7 @@
         <v>35</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>35</v>
@@ -1123,19 +1153,19 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>35</v>
+      <c r="C23" s="5">
+        <v>40977</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>35</v>
+        <v>51</v>
+      </c>
+      <c r="E23" s="5">
+        <v>40983</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>28</v>
@@ -1152,23 +1182,23 @@
         <v>40954</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>35</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>37</v>
@@ -1178,14 +1208,15 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1"/>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1240,4 +1271,91 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update to Schedule.xlsx And re-adding Actions/Functions/Sops
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
   <si>
     <t>Item</t>
   </si>
@@ -192,9 +192,6 @@
     <t>pablo</t>
   </si>
   <si>
-    <t>MarkS (MikeP - 2 initial sections)</t>
-  </si>
-  <si>
     <t>JSON (verbose version)</t>
   </si>
   <si>
@@ -250,6 +247,12 @@
   </si>
   <si>
     <t>&lt;some base&gt;/odata</t>
+  </si>
+  <si>
+    <t>OData Core – Appendix  – 2 initial sections</t>
+  </si>
+  <si>
+    <t>ongoing</t>
   </si>
 </sst>
 </file>
@@ -358,11 +361,53 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -383,6 +428,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -390,7 +442,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -691,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,7 +822,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="5">
-        <v>40956</v>
+        <v>40960</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>56</v>
@@ -808,8 +867,8 @@
       <c r="D5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="5">
-        <v>40956</v>
+      <c r="E5" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>55</v>
@@ -822,14 +881,14 @@
       <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="5">
-        <v>40956</v>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="5">
-        <v>40959</v>
+        <v>40961</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>55</v>
@@ -842,14 +901,14 @@
       <c r="B7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="5">
-        <v>40956</v>
+      <c r="C7" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E7" s="5">
-        <v>40959</v>
+        <v>40960</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>55</v>
@@ -863,13 +922,13 @@
         <v>12</v>
       </c>
       <c r="C8" s="5">
-        <v>40957</v>
+        <v>40961</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="5">
-        <v>40959</v>
+        <v>40962</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>28</v>
@@ -883,13 +942,13 @@
         <v>12</v>
       </c>
       <c r="C9" s="5">
-        <v>40957</v>
+        <v>40960</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E9" s="5">
-        <v>40952</v>
+        <v>40961</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>55</v>
@@ -949,7 +1008,7 @@
         <v>16</v>
       </c>
       <c r="E12" s="5">
-        <v>40959</v>
+        <v>40960</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>55</v>
@@ -963,13 +1022,13 @@
         <v>20</v>
       </c>
       <c r="C13" s="10">
-        <v>40956</v>
+        <v>40959</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="10">
-        <v>40959</v>
+        <v>40964</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="9" t="s">
@@ -983,8 +1042,8 @@
       <c r="B14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="5">
-        <v>40956</v>
+      <c r="C14" s="10">
+        <v>40959</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>16</v>
@@ -1003,8 +1062,8 @@
       <c r="B15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="5">
-        <v>40956</v>
+      <c r="C15" s="10">
+        <v>40959</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>16</v>
@@ -1018,68 +1077,68 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="C16" s="5">
-        <v>40968</v>
+        <v>40960</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>36</v>
       </c>
       <c r="E16" s="5">
-        <v>40971</v>
+        <v>40961</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="7" t="s">
+    <row r="17" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C17" s="10">
         <v>40968</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="10">
+        <v>40971</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="10">
+        <v>40968</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="10">
-        <v>40959</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="10">
-        <v>40962</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>47</v>
@@ -1091,7 +1150,7 @@
         <v>52</v>
       </c>
       <c r="E19" s="10">
-        <v>40962</v>
+        <v>40967</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="9" t="s">
@@ -1100,19 +1159,19 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>47</v>
       </c>
       <c r="C20" s="10">
+        <v>40967</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="10">
         <v>40968</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>35</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="9" t="s">
@@ -1120,60 +1179,61 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="5">
-        <v>40963</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="5">
-        <v>40966</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>55</v>
+      <c r="A21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="10">
+        <v>40970</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="10">
+        <v>40974</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>35</v>
+        <v>16</v>
+      </c>
+      <c r="C22" s="5">
+        <v>40963</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>35</v>
+        <v>49</v>
+      </c>
+      <c r="E22" s="5">
+        <v>40966</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="5">
-        <v>40977</v>
+      <c r="C23" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="5">
-        <v>40983</v>
+      <c r="E23" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>28</v>
@@ -1181,54 +1241,90 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="5">
+        <v>40977</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="5">
+        <v>40983</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B25" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B29" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="5">
-        <v>40953</v>
+      <c r="C29" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1"/>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+  <conditionalFormatting sqref="G1:G16 G18:G1048576">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C16 C18:C1048576">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="G17">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"Not Started"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
@@ -1303,68 +1399,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>60</v>
-      </c>
       <c r="C1" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
         <v>61</v>
       </c>
-      <c r="B2" t="s">
-        <v>62</v>
-      </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
         <v>63</v>
       </c>
-      <c r="B3" t="s">
-        <v>64</v>
-      </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
         <v>66</v>
       </c>
-      <c r="B5" t="s">
-        <v>67</v>
-      </c>
       <c r="C5" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated schedule with my latest work Comments on Extensibility Sections
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="77">
   <si>
     <t>Item</t>
   </si>
@@ -250,9 +250,6 @@
   </si>
   <si>
     <t>OData Core – Appendix  – 2 initial sections</t>
-  </si>
-  <si>
-    <t>ongoing</t>
   </si>
 </sst>
 </file>
@@ -361,7 +358,226 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="38">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -718,7 +934,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,7 +1049,7 @@
         <v>36</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>55</v>
@@ -872,8 +1088,8 @@
       <c r="D7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="5">
-        <v>40960</v>
+      <c r="E7" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>55</v>
@@ -1053,8 +1269,8 @@
       <c r="D16" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="5">
-        <v>40961</v>
+      <c r="E16" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>28</v>
@@ -1263,35 +1479,48 @@
   </sheetData>
   <autoFilter ref="A1:F1"/>
   <conditionalFormatting sqref="G1:G16 G18:G1048576">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="9" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C16 C18:C1048576">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E25">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+      <formula>"DONE"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"DONE"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
This time with a decent format for DONE!
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -358,11 +358,26 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="23">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -453,128 +468,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -934,7 +827,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,48 +1372,51 @@
   </sheetData>
   <autoFilter ref="A1:F1"/>
   <conditionalFormatting sqref="G1:G16 G18:G1048576">
-    <cfRule type="cellIs" dxfId="20" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C16 C18:C1048576">
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E25">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"DONE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"DONE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Incorporated comments in Extensibility section.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -747,7 +747,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,7 +905,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1086,7 +1086,7 @@
         <v>10</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1107,7 +1107,7 @@
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="9" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated my estimates - I've slipped about a week.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="76">
   <si>
     <t>Item</t>
   </si>
@@ -160,9 +160,6 @@
   </si>
   <si>
     <t>URI glossary terms (service root, etc)</t>
-  </si>
-  <si>
-    <t>AlexJ</t>
   </si>
   <si>
     <t>URI - Addressing conventions (consider using odata.org as base)</t>
@@ -747,7 +744,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,13 +816,13 @@
         <v>40962</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>35</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -862,10 +859,10 @@
         <v>36</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -885,7 +882,7 @@
         <v>40961</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -945,7 +942,7 @@
         <v>40967</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -959,7 +956,7 @@
         <v>35</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>35</v>
@@ -985,7 +982,7 @@
         <v>40976</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1005,7 +1002,7 @@
         <v>40960</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1026,7 +1023,7 @@
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1046,7 +1043,7 @@
         <v>40964</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1066,12 +1063,12 @@
         <v>40964</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>16</v>
@@ -1107,7 +1104,7 @@
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1135,34 +1132,34 @@
         <v>46</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="C19" s="10">
-        <v>40963</v>
+        <v>40977</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" s="10">
         <v>40967</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="C20" s="10">
-        <v>40967</v>
+        <v>40981</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="10">
         <v>40968</v>
@@ -1177,10 +1174,10 @@
         <v>33</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="C21" s="10">
-        <v>40970</v>
+        <v>40984</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>9</v>
@@ -1204,13 +1201,13 @@
         <v>40963</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E22" s="5">
         <v>40966</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1224,7 +1221,7 @@
         <v>35</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>35</v>
@@ -1235,7 +1232,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>9</v>
@@ -1244,7 +1241,7 @@
         <v>40977</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" s="5">
         <v>40983</v>
@@ -1270,17 +1267,17 @@
         <v>35</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>37</v>
@@ -1409,68 +1406,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>59</v>
-      </c>
       <c r="C1" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
         <v>60</v>
       </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
         <v>65</v>
       </c>
-      <c r="B5" t="s">
-        <v>66</v>
-      </c>
       <c r="C5" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated based on 3/7 sync up.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="77">
   <si>
     <t>Item</t>
   </si>
@@ -147,9 +147,6 @@
     <t>MarkS</t>
   </si>
   <si>
-    <t>MFlasko</t>
-  </si>
-  <si>
     <t>JSON Format (efficient format) + its vocab</t>
   </si>
   <si>
@@ -244,6 +241,15 @@
   </si>
   <si>
     <t>OData Core – Appendix  – 2 initial sections</t>
+  </si>
+  <si>
+    <t>mflasko/Alex</t>
+  </si>
+  <si>
+    <t>Done? Ready to check in? Asad to follow up…</t>
+  </si>
+  <si>
+    <t>Asad: check w/pablo to get a review date.</t>
   </si>
 </sst>
 </file>
@@ -741,7 +747,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,13 +799,13 @@
         <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="E2" s="5">
         <v>40986</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -813,18 +819,21 @@
         <v>40962</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>34</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="H3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>13</v>
@@ -856,10 +865,10 @@
         <v>35</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -879,7 +888,10 @@
         <v>40961</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="H6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -921,6 +933,9 @@
       <c r="G8" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="H8" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -939,7 +954,10 @@
         <v>40967</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="H9" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -949,11 +967,11 @@
       <c r="B10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>34</v>
+      <c r="C10" s="5">
+        <v>40987</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>34</v>
@@ -970,16 +988,16 @@
         <v>9</v>
       </c>
       <c r="C11" s="5">
-        <v>40970</v>
+        <v>40976</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E11" s="5">
-        <v>40976</v>
+        <v>40981</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -999,7 +1017,7 @@
         <v>40980</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1020,7 +1038,7 @@
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1040,7 +1058,7 @@
         <v>40980</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1060,12 +1078,12 @@
         <v>40980</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>16</v>
@@ -1083,7 +1101,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>25</v>
       </c>
@@ -1091,20 +1109,20 @@
         <v>41</v>
       </c>
       <c r="C17" s="10">
-        <v>40968</v>
+        <v>40982</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>35</v>
       </c>
       <c r="E17" s="10">
-        <v>40971</v>
+        <v>40987</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1112,7 +1130,7 @@
         <v>41</v>
       </c>
       <c r="C18" s="10">
-        <v>40968</v>
+        <v>40987</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>34</v>
@@ -1124,9 +1142,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>20</v>
@@ -1135,19 +1153,19 @@
         <v>40977</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="10">
-        <v>40967</v>
+        <v>49</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>20</v>
@@ -1156,17 +1174,17 @@
         <v>40981</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="10">
-        <v>40968</v>
+        <v>49</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>32</v>
       </c>
@@ -1179,15 +1197,15 @@
       <c r="D21" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="10">
-        <v>40974</v>
+      <c r="E21" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -1198,15 +1216,15 @@
         <v>40977</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>9</v>
@@ -1215,7 +1233,7 @@
         <v>34</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>34</v>
@@ -1224,18 +1242,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="5">
-        <v>40977</v>
+        <v>40984</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="5">
         <v>40983</v>
@@ -1244,7 +1262,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1261,17 +1279,20 @@
         <v>34</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="H25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>52</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>36</v>
@@ -1400,68 +1421,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>57</v>
-      </c>
       <c r="C1" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="s">
-        <v>59</v>
-      </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
         <v>60</v>
       </c>
-      <c r="B3" t="s">
-        <v>61</v>
-      </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
         <v>63</v>
       </c>
-      <c r="B5" t="s">
-        <v>64</v>
-      </c>
       <c r="C5" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished draft of service document section and updated schedule
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="77">
   <si>
     <t>Item</t>
   </si>
@@ -747,7 +747,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,8 +815,8 @@
       <c r="B3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="5">
-        <v>40962</v>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>53</v>
@@ -921,8 +921,8 @@
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5">
-        <v>40966</v>
+      <c r="C8" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>16</v>
@@ -944,8 +944,8 @@
       <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="5">
-        <v>40966</v>
+      <c r="C9" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Updated with progress on CUD, including separating out named streams.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="78">
   <si>
     <t>Item</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>Asad: check w/pablo to get a review date.</t>
+  </si>
+  <si>
+    <t>CUD for named streams</t>
   </si>
 </sst>
 </file>
@@ -360,10 +363,9 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -375,9 +377,10 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -744,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,8 +990,8 @@
       <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="5">
-        <v>40976</v>
+      <c r="C11" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>35</v>
@@ -1285,19 +1288,40 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+    <row r="26" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="10">
+        <v>40981</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B30" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1335,20 +1359,20 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E25">
+  <conditionalFormatting sqref="E2:E26">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"DONE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"In Progress"</formula>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Done"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"DONE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Done"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"In Progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated for Json verbose status.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="13612"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dd\new_spec\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20160" windowHeight="8100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27750" windowHeight="14385"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="78">
   <si>
     <t>Item</t>
   </si>
@@ -455,6 +460,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -750,7 +758,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,8 +1260,8 @@
       <c r="B24" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="5">
-        <v>40984</v>
+      <c r="C24" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Updated list of todo items
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="13612"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dd\new_spec\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27750" windowHeight="14385"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="82">
   <si>
     <t>Item</t>
   </si>
@@ -176,12 +171,6 @@
     <t>Mflasko</t>
   </si>
   <si>
-    <t>Work Items</t>
-  </si>
-  <si>
-    <t>Create table of doc names and short ref tags</t>
-  </si>
-  <si>
     <t>In Progress</t>
   </si>
   <si>
@@ -258,6 +247,24 @@
   </si>
   <si>
     <t>CUD for named streams</t>
+  </si>
+  <si>
+    <t>Extract ABNF into separate doc</t>
+  </si>
+  <si>
+    <t>Spatial todos in UriConventions doc</t>
+  </si>
+  <si>
+    <t>Move uri query semantic/syntax as appropriate</t>
+  </si>
+  <si>
+    <t>Alex / MikeP</t>
+  </si>
+  <si>
+    <t>Create initial terminology section</t>
+  </si>
+  <si>
+    <t>Later</t>
   </si>
 </sst>
 </file>
@@ -755,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,13 +817,13 @@
         <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E2" s="5">
         <v>40986</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -830,16 +837,16 @@
         <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>34</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -899,10 +906,10 @@
         <v>40961</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -945,7 +952,7 @@
         <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -965,10 +972,10 @@
         <v>40967</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -979,7 +986,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="5">
-        <v>40987</v>
+        <v>40997</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>48</v>
@@ -1008,7 +1015,7 @@
         <v>40981</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1028,7 +1035,7 @@
         <v>40980</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1049,7 +1056,7 @@
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1069,7 +1076,7 @@
         <v>40980</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1089,12 +1096,12 @@
         <v>40980</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>16</v>
@@ -1120,7 +1127,7 @@
         <v>41</v>
       </c>
       <c r="C17" s="10">
-        <v>40982</v>
+        <v>40994</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>35</v>
@@ -1130,7 +1137,7 @@
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1141,7 +1148,7 @@
         <v>41</v>
       </c>
       <c r="C18" s="10">
-        <v>40987</v>
+        <v>40994</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>34</v>
@@ -1160,8 +1167,8 @@
       <c r="B19" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="10">
-        <v>40977</v>
+      <c r="C19" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>49</v>
@@ -1171,7 +1178,7 @@
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1181,8 +1188,8 @@
       <c r="B20" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="10">
-        <v>40981</v>
+      <c r="C20" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>49</v>
@@ -1202,8 +1209,8 @@
       <c r="B21" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="10">
-        <v>40984</v>
+      <c r="C21" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>9</v>
@@ -1223,31 +1230,31 @@
       <c r="B22" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="5">
-        <v>40977</v>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>46</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>34</v>
+      <c r="E23" s="5">
+        <v>40983</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>27</v>
@@ -1255,83 +1262,148 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="B24" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="C25" s="10">
+        <v>40995</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="5">
+        <v>40995</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="10">
+        <v>40996</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="10">
+        <v>40997</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="10">
+        <v>40994</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="11"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="9"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="5">
-        <v>40983</v>
-      </c>
-      <c r="G24" s="4" t="s">
+      <c r="E31" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H25" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="10">
-        <v>40981</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>10</v>
-      </c>
+    <row r="32" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="11"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1"/>
@@ -1367,7 +1439,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E26">
+  <conditionalFormatting sqref="E2:E25 E31:E32">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"DONE"</formula>
     </cfRule>
@@ -1453,68 +1525,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Split the ABNF out into its own document.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="13612"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dd\new_spec\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27750" windowHeight="14385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18210" windowHeight="10185"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="82">
   <si>
     <t>Item</t>
   </si>
@@ -765,7 +770,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,8 +1295,8 @@
       <c r="B25" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="10">
-        <v>40995</v>
+      <c r="C25" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>35</v>
@@ -1311,8 +1316,8 @@
       <c r="B26" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="5">
-        <v>40995</v>
+      <c r="C26" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>27</v>

</xml_diff>